<commit_message>
Test added test on the hsize handling.
- Fully randomized.
</commit_message>
<xml_diff>
--- a/Test Plans.xlsx
+++ b/Test Plans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Teo Sei Hau\Project\Git\AMBA-AHB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B4529D-277B-4B82-97EE-213AF2B2DB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CD2509-3D48-4CD1-95AF-2B71D479C693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" xr2:uid="{3DFF275C-F6BB-4F42-B6D6-D929A6041B9E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Test Plan</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>1 Write + 1 Read to the same address</t>
+  </si>
+  <si>
+    <t>Multiple Write + Multiple Read txns with hsize, haddr same for each set of txns, to test on hsize handling.</t>
   </si>
 </sst>
 </file>
@@ -535,7 +538,7 @@
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -577,9 +580,15 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>

</xml_diff>

<commit_message>
Update test plans for write strobe feature.
</commit_message>
<xml_diff>
--- a/Test Plans.xlsx
+++ b/Test Plans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Teo Sei Hau\Project\Git\AMBA-AHB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CD2509-3D48-4CD1-95AF-2B71D479C693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEAA2EB-CC78-46B4-BCDC-D672CCEAAADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" xr2:uid="{3DFF275C-F6BB-4F42-B6D6-D929A6041B9E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Test Plan</t>
   </si>
@@ -93,9 +93,6 @@
     <t>pstate = ACCESS</t>
   </si>
   <si>
-    <t>Transfer Mode</t>
-  </si>
-  <si>
     <t>Basic transfers</t>
   </si>
   <si>
@@ -103,6 +100,24 @@
   </si>
   <si>
     <t>Multiple Write + Multiple Read txns with hsize, haddr same for each set of txns, to test on hsize handling.</t>
+  </si>
+  <si>
+    <t>Testing Feature</t>
+  </si>
+  <si>
+    <t>Write Strobe</t>
+  </si>
+  <si>
+    <t>Full word write: Test a 32-bit data bus with all strobes active (HWSTRB = 1111).</t>
+  </si>
+  <si>
+    <t>Sparse Write: Test a 32-bit data bus with only selected strobes active (HWSTRB = 1010 updates only bytes 0 and 2).</t>
+  </si>
+  <si>
+    <t>No Write (All Strobes Inactive)</t>
+  </si>
+  <si>
+    <t>Cross feature with hsize (HSIZE = HALF_WORD, HWSTRB = 0001)</t>
   </si>
 </sst>
 </file>
@@ -535,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729EC54C-6585-402F-8223-56F2D92B6FBF}">
-  <dimension ref="B2:D6"/>
+  <dimension ref="B2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -546,7 +561,7 @@
     <col min="1" max="1" width="8.7265625" style="2"/>
     <col min="2" max="2" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="104.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="109" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.7265625" style="2"/>
   </cols>
@@ -562,7 +577,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>1</v>
@@ -573,10 +588,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
@@ -584,16 +599,55 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
+      <c r="B6" s="4">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="4">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="4">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated to handle IDLE and BUSY transactions
</commit_message>
<xml_diff>
--- a/Test Plans.xlsx
+++ b/Test Plans.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Teo Sei Hau\Project\Git\AMBA-AHB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEAA2EB-CC78-46B4-BCDC-D672CCEAAADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A87845-B5A0-4517-B06F-0C0C4B8D5A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" xr2:uid="{3DFF275C-F6BB-4F42-B6D6-D929A6041B9E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Test Plan</t>
   </si>
@@ -51,57 +51,12 @@
     <t>Coverage Plan</t>
   </si>
   <si>
-    <t>Coverage No</t>
-  </si>
-  <si>
-    <t>Conditions</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>IDLE State</t>
-  </si>
-  <si>
-    <t>pstate = IDLE</t>
-  </si>
-  <si>
-    <t>Setup State</t>
-  </si>
-  <si>
-    <t>pstate = SETUP</t>
-  </si>
-  <si>
-    <t>Write Access</t>
-  </si>
-  <si>
-    <t>pstate = ACCESS, pwrite = 1</t>
-  </si>
-  <si>
-    <t>Read Access</t>
-  </si>
-  <si>
-    <t>pstate = ACCESS, pwrite = 0</t>
-  </si>
-  <si>
-    <t>state_cp</t>
-  </si>
-  <si>
-    <t>state_write_cross</t>
-  </si>
-  <si>
-    <t>pstate = ACCESS</t>
-  </si>
-  <si>
     <t>Basic transfers</t>
   </si>
   <si>
     <t>1 Write + 1 Read to the same address</t>
   </si>
   <si>
-    <t>Multiple Write + Multiple Read txns with hsize, haddr same for each set of txns, to test on hsize handling.</t>
-  </si>
-  <si>
     <t>Testing Feature</t>
   </si>
   <si>
@@ -118,6 +73,24 @@
   </si>
   <si>
     <t>Cross feature with hsize (HSIZE = HALF_WORD, HWSTRB = 0001)</t>
+  </si>
+  <si>
+    <t>Cross Feature</t>
+  </si>
+  <si>
+    <t>IDLE Transfer</t>
+  </si>
+  <si>
+    <t>Send an IDLE transfer and verify that no read/write occurs and subordinate responds with OKAY.</t>
+  </si>
+  <si>
+    <t>BUSY Transfer</t>
+  </si>
+  <si>
+    <t>Send an BUSY transfer and verify that no read/write occurs and subordinate responds with OKAY.</t>
+  </si>
+  <si>
+    <t>Multiple Write + Multiple Read txns with hsize, haddr same for each set of txns, with other fields randomize.</t>
   </si>
 </sst>
 </file>
@@ -550,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729EC54C-6585-402F-8223-56F2D92B6FBF}">
-  <dimension ref="B2:D9"/>
+  <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -577,7 +550,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>1</v>
@@ -588,10 +561,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
@@ -599,10 +572,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
@@ -610,10 +583,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
@@ -621,10 +594,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
@@ -632,10 +605,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
@@ -643,10 +616,32 @@
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>26</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="4">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -659,7 +654,7 @@
   <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -682,104 +677,52 @@
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="2:4" ht="21" x14ac:dyDescent="0.5">
-      <c r="B4" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="B4" s="7"/>
       <c r="C4" s="3"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="4">
-        <v>2</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="4">
-        <v>3</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="4">
-        <v>4</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="11" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B11" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="B11" s="7"/>
     </row>
     <row r="12" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="4">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B14" s="4">
-        <v>2</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed logical error for write operations
- haddr signal should be aligned with hsize (e.g. for word transfer, haddr % 4 == 0);
- hwstrb should be compatible with hsize and haddr (Masking operation supported!)
</commit_message>
<xml_diff>
--- a/Test Plans.xlsx
+++ b/Test Plans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Teo Sei Hau\Project\Git\AMBA-AHB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A87845-B5A0-4517-B06F-0C0C4B8D5A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC031C80-A0E7-4344-820D-CFD0F73DD01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" xr2:uid="{3DFF275C-F6BB-4F42-B6D6-D929A6041B9E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>Test Plan</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Coverage Plan</t>
   </si>
   <si>
-    <t>Basic transfers</t>
-  </si>
-  <si>
     <t>1 Write + 1 Read to the same address</t>
   </si>
   <si>
@@ -91,6 +88,42 @@
   </si>
   <si>
     <t>Multiple Write + Multiple Read txns with hsize, haddr same for each set of txns, with other fields randomize.</t>
+  </si>
+  <si>
+    <t>Burst Transfers</t>
+  </si>
+  <si>
+    <t>Basic Transfers</t>
+  </si>
+  <si>
+    <t>Incrementing Burst (INCR): Check that addresses increment correctly and stay within the subordinate’s addressable range.</t>
+  </si>
+  <si>
+    <t>WRAP4 (HBURST = 0b010): Verify that the address wraps correctly at the boundary</t>
+  </si>
+  <si>
+    <t>WRAP8 (HBURST = 0b100)</t>
+  </si>
+  <si>
+    <t>WRAP16 (HBURST = 0b110)</t>
+  </si>
+  <si>
+    <t>INCR4 (HBURST = 0b011)</t>
+  </si>
+  <si>
+    <t>INCR8 (HBURST = 0b101)</t>
+  </si>
+  <si>
+    <t>INCR16 (HBURST = 0b111)</t>
+  </si>
+  <si>
+    <t>Edge Cases:Burst with minimum transfer size (HSIZE = BYTE)</t>
+  </si>
+  <si>
+    <t>Edge Cases:Burst with maximum transfer size (HSIZE = WORD)</t>
+  </si>
+  <si>
+    <t>Edge Cases:Early burst termination</t>
   </si>
 </sst>
 </file>
@@ -143,7 +176,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -166,11 +199,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -189,6 +235,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729EC54C-6585-402F-8223-56F2D92B6FBF}">
-  <dimension ref="B2:D11"/>
+  <dimension ref="B2:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -550,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>1</v>
@@ -561,10 +608,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
@@ -572,10 +619,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
@@ -583,10 +630,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
@@ -594,10 +641,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
@@ -605,10 +652,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
@@ -616,10 +663,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
@@ -627,10 +674,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
@@ -638,10 +685,120 @@
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="4">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
         <v>12</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>17</v>
+      <c r="C15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="4">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="4">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="4">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="4">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="4">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="4">
+        <v>18</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.5: Added Burst handling
</commit_message>
<xml_diff>
--- a/Test Plans.xlsx
+++ b/Test Plans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Teo Sei Hau\Project\Git\AMBA-AHB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC031C80-A0E7-4344-820D-CFD0F73DD01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09082F6B-AE38-412F-B35E-AC831A18EAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" xr2:uid="{3DFF275C-F6BB-4F42-B6D6-D929A6041B9E}"/>
+    <workbookView xWindow="340" yWindow="2240" windowWidth="17820" windowHeight="11770" xr2:uid="{3DFF275C-F6BB-4F42-B6D6-D929A6041B9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Stimulus" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Test Plan</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>Edge Cases:Burst with minimum transfer size (HSIZE = BYTE)</t>
-  </si>
-  <si>
-    <t>Edge Cases:Burst with maximum transfer size (HSIZE = WORD)</t>
   </si>
   <si>
     <t>Edge Cases:Early burst termination</t>
@@ -570,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729EC54C-6585-402F-8223-56F2D92B6FBF}">
-  <dimension ref="B2:D21"/>
+  <dimension ref="B2:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="B18" sqref="B18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -784,20 +781,9 @@
         <v>17</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="4">
-        <v>18</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>